<commit_message>
refine & add deepeval
</commit_message>
<xml_diff>
--- a/search_results.xlsx
+++ b/search_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,42 +467,42 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Text Search</t>
+          <t>Text</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Text Search</t>
+          <t>Text</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Vector Search</t>
+          <t>Vector</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Vector Search</t>
+          <t>Vector</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Hybrid Search</t>
+          <t>Hybrid</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Hybrid Search</t>
+          <t>Hybrid</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Semantic Hybrid Search</t>
+          <t>Hybrid Semantic</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Semantic Hybrid Search</t>
+          <t>Hybrid Semantic</t>
         </is>
       </c>
     </row>
@@ -513,28 +513,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.919112</v>
+        <v>2.4517398</v>
       </c>
       <c r="C3" t="n">
-        <v>0.79283696</v>
+        <v>2.1927474</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8529292000000001</v>
+        <v>0.8692876</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8396100399999999</v>
+        <v>0.8572363</v>
       </c>
       <c r="F3" t="n">
-        <v>0.03333333507180214</v>
+        <v>0.03279569745063782</v>
       </c>
       <c r="G3" t="n">
-        <v>0.03201844170689583</v>
+        <v>0.03125763311982155</v>
       </c>
       <c r="H3" t="n">
-        <v>0.03333333507180214</v>
+        <v>0.0307511743158102</v>
       </c>
       <c r="I3" t="n">
-        <v>0.01388888899236917</v>
+        <v>0.03083491325378418</v>
       </c>
     </row>
     <row r="4">
@@ -550,56 +550,290 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>3.277726650238037</v>
+        <v>3.594822406768799</v>
       </c>
       <c r="I4" t="n">
-        <v>2.306142807006836</v>
+        <v>2.793275117874146</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
+          <t>Contextual Precision</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Contextual Precision Reason</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>The score is 0.00 because the provided node in the retrieval context, which is ranked first, discusses "urbanization trends and the definition of a city" but fails to answer the question about which city is the biggest in the world. This node should be ranked lower as it is irrelevant to the specific information requested. There are no relevant nodes ranked higher to justify a higher score.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>The score is 1.00 because all relevant nodes containing the necessary information, specifically the node stating "Japan Tokyo Metropolitan area 34 450 38 140 37 190", are ranked at the top. This node, ranked first, precisely answers the input question by indicating that Tokyo is the biggest city mentioned, demonstrating perfect contextual precision. There are no irrelevant nodes ranked above this pertinent information.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>The score is 1.00 because the first node in the retrieval context provides the precise information needed, stating "Despite a projected decline of nearly 1 million inhabitants, Tokyo is expected to remain the world’s largest city in 2030..." which straightaway addresses the query about the biggest city in the world. This indicates a perfect ranking with all relevant nodes placed above any irrelevant ones.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>The score is 0.00 because the nodes in the retrieval context that are ranked highest fail to provide specific information about the largest city in the world. The first node does not directly indicate which city is the biggest, as it merely lists cities and their populations without clarification. The second node discusses population growth projections and regional distribution but omits details on the present largest city. Both nodes should be ranked lower due to their lack of pertinent information, as indicated by their explanations that they do "not directly indicate which is the biggest city in the world" and "does not specify the current biggest city."</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>The score is 0.00 because the first node in the retrieval context, which should contain the most relevant information, focuses on "urbanization and the importance of understanding city populations" but fails to answer the question about "which is the biggest city in the world." Since no other nodes are provided, and this node does not provide the specific information required, it's categorized as irrelevant and should be ranked lower. Consequently, there are no relevant nodes ranked above the irrelevant ones, which justifies the lowest possible precision score.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>The score is 0.00 because the node in the retrieval context, which is ranked first, is not relevant to the input question about the biggest city in the world. It discusses "population projections and the percentage of people living in cities of various sizes," but fails to mention any specific city, let alone identifying which is the largest. Therefore, this irrelevant node should be ranked lower than a relevant node that directly answers the question.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>The score is 1.00 because all relevant nodes are ranked above any irrelevant nodes. Specifically, the first node in the retrieval context provides the exact information needed, stating "Despite a projected decline... Tokyo is expected to remain the world’s largest city in 2030," which perfectly supports the answer that Tokyo, Japan is the biggest city in the world. Since there are no irrelevant nodes ranked higher than this highly relevant node, the contextual precision is at its maximum. Great job on precision!</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>The score is 0.00 because the information provided in the first node of the retrieval context does not address the query about the biggest city in the world. It only lists "various cities in Southern and Western Europe with population figures and rates of change" and fails to mention "Tokyo" or identify any city as the biggest. Therefore, relevant nodes that should contain the necessary information for the query are not ranked above this irrelevant node.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Contextual Recall</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Contextual Recall Reason</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>The score is 0.00 because there's absolutely no mention of Tokyo, Japan or any information about the biggest city in the world in the nodes in the retrieval context, which directly corresponds to the absence of supportive content for the expected output statement.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>The score is 1.00 because every part of the expected output is perfectly reflected in the retrieval context, specifically within the 9th node that provides data on Tokyo's population, thereby confirming its status as the biggest city. Great job on achieving full alignment!</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>The score is 1.00 because the 2nd node in the retrieval context clearly states Tokyo's status as the world's largest city, directly supporting the sentence in the expected output. Great job on the precise match!</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>The score is 0.00 because the sentence in the expected output (sentence 1) that claims Tokyo, Japan is the biggest city in the world is not supported by any information from the nodes in the retrieval context.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>The score is 0.00 because none of the nodes in the retrieval context provide information about Tokyo, Japan, or its distinction as the biggest city in the world, as claimed in sentence 1 of the expected output.</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>The score is 0.00 because sentence 1 in the expected output, which claims that Tokyo, Japan is the biggest city in the world, has no corresponding information in any node in the retrieval context that supports this statement.</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>The score is 1.00 because every detail in the expected output is perfectly aligned with the information from the 1st node in the retrieval context, highlighting Tokyo's status as the largest city. Great job on the accuracy!</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>The score is 0.00 because sentence 1 in the expected output refers to Tokyo as the biggest city in the world, yet none of the nodes in the retrieval context provide information to support this statement.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Contextual Relevancy</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Contextual Relevancy Reason</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>The score is 0.00 because the context fails to directly answer the specific question "What is the biggest city in the world?" and instead provides only general background on urbanization without identifying the largest city.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>The score is 1.00 because the retrieval context aligns perfectly with the input, ensuring the most accurate and relevant information is provided. Great job on maintaining context!</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>The score is 1.00 because the retrieval context perfectly aligns with the input, ensuring the most accurate and relevant information is provided. Great job on maintaining high contextual relevance!</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>The score is 0.00 because the context fails to identify the "biggest city in the world" by any definitive measure like population or area, as indicated by the provided reasons for irrelevancy.</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>The score is 0.00 because the context does not specify which city is the biggest in the world, despite providing general urbanization information and global city statistics.</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>The score is 0.00 because the provided context fails to specify which city is the 'biggest', either by population or area, which is the exact information needed to answer the question "What is the biggest city in the world?". General statistics on urban population growth and the distribution of megacities do not contribute to identifying a specific city, as indicated in the reasons for irrelevancy.</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>The score is 1.00 because the input was clear and no reasons for irrelevancy were provided, indicating a perfect match in context. Great job!</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>The score is 0.00 because the context fails to identify the biggest city in the world, directly omitting the key information asked for in the input.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
           <t>Content</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>The World’s Cities in 2016 United Nations Data Booklet file:V:\PEP-Section\WUP2014\2016%20Data%20Booklet\Charts%20and%20Images\4_Urbanization_BusanRepublic%20of%20Korea2011UNPhoto_Kibae%20Park_03022015.jpg ii The World’s Cities in 2016 In 2016, an estimated 54.5 per cent of the world’s population lived in urban settlements. By 2030, urban areas are projected to house 60 per cent of people globally and one in every three people will live in cities with at least half a million inhabitants. Understanding the key trends in urbanization likely to unfold over the coming years is crucial to the implementation of the 2030 Agenda for Sustainable Development and for efforts to forge a new framework of ur- ban development during the Habitat III confer- ence scheduled to be held in Quito, Ecuador in October 2016. This data booklet highlights current and future trajectories of populations in cities around the globe, drawing on population estimates and projections published in World Urbanization Prospects: The 2014 Revision. All information is available at www.unpopulation.org. Suggested citation: United Nations, Department of Economic and Social Affairs, Population Di- vision (2016). The World’s Cities in 2016 – Data Booklet (ST/ESA/ SER.A/392). Cover photo: Copyright © UN Photo/Kibae Park 1The World’s Cities in 2016 What is a City? Most people can agree that cities are places where large numbers of people live and work; they are hubs of government, commerce and transportation. But how best to define the geographical limits of a city is a matter of some debate. So far, no standardized international criteria exist for determining the boundaries of a city and often multiple different boundary definitions are available for any given city. One type of definition, sometimes referred to as the “city proper”, describes a city according to an administrative boundary. A second approach, termed the “ur-</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1.4 0.2 0.3 China, Hong Kong SAR Hong Kong Urban Agglomeration 6 835 7 365 7 885 0.5 0.5 100.0 100.0 Dem. People’s Rep. of Korea P’yongyang City Proper 2 777 2 872 3 277 0.2 0.9 11.4 18.6 Japan Chukyo M.M.A. (Nagoya) Metropolitan area 8 740 9 434 9 304 0.5 -0.1 7.5 7.9 Japan Hiroshima Metropolitan area 2 044 2 180 2 213 0.4 0.1 1.7 1.8 Japan Kinki M.M.A. (Osaka) Metropolitan area 18 660 20 337 19 976 0.5 -0.1 16.1 17.1 Japan Kitakyushu-Fukuoka M.M.A. Metropolitan area 5 421 5 494 5 355 0.1 -0.2 4.3 4.6 Japan Sapporo Metropolitan area 2 508 2 564 2 542 0.1 -0.1 2.0 2.2 Japan Sendai Metropolitan area 2 184 2 071 2 012 -0.3 -0.2 1.6 1.7 Japan Shizuoka-Hamamatsu M.M.A. Metropolitan area 1 217 3 493 3 934 6.6 0.8 2.8 2.9 Japan Tokyo Metropolitan area 34 450 38 140 37 190 0.6 -0.2 30.1 32.1 Mongolia Ulaanbaatar City Proper 765 1 421 1 850 3.9 1.9 47.9 65.8 Republic of Korea Busan City Proper 3 594 3 200 3 264 -0.7 0.1 6.4 7.8 15The World’s Cities in 2016 City population (thousands) Average annual rate of change (percentage) City population as a proportion of the country or area’s total or urban population in 2016 (percentage) Country or area City Statistical Concepts 2000 2016 2030 2000-2016 2016-2030 Total population Urban population Republic of Korea Changwon Urban Agglomeration 1 077 1 036 1 090 -0.2 0.4 2.1 2.5 Republic of Korea Daegu City Proper 2 323 2 241 2 328 -0.2 0.3 4.5 5.4 Republic of Korea Daejon City Proper 1 354 1 578 1 711 1.0 0.6 3.2 3.8 Republic of Korea Gwangju City Proper 1 343 1 550 1 682 0.9 0.6 3.1 3.8 Republic of Korea Incheon City Proper 2 371 2 711 2 919 0.8 0.5 5.4 6.6</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
         <is>
           <t>countries. They include: Lahore, Pakistan Hyderabad, India Bogotá, Colombia Johannesburg, South Africa Bangkok, Thailand Dar es Salaam, Tanzania Ahmanabad, India Luanda, Angola Ho Chi Minh City, Viet Nam and Chungdu, China. Despite a projected decline of nearly 1 million inhabitants, Tokyo is ex- pected to remain the world’s largest city in 2030, followed by Delhi, which is projected to add nearly 10 million people between 2016 and 2030. Rank City, Country Population in 2016 (thousands) City, Country Population in 2030 (thousands) 1 Tokyo, Japan 38 140 Tokyo, Japan 37 190 2 Delhi, India 26 454 Delhi, India 36 060 3 Shanghai, China 24 484 Shanghai, China 30 751 4 Mumbai (Bombay), India 21 357 Mumbai (Bombay), India 27 797 5 São Paulo, Brazil 21 297 Beijing, China 27 706 6 Beijing, China 21 240 Dhaka, Bangladesh 27 374 7 Ciudad de México (Mexico City), Mexico 21 157 Karachi, Pakistan 24 838 8 Kinki M.M.A. (Osaka), Japan 20 337 Al-Qahirah (Cairo), Egypt 24 502 9 Al-Qahirah (Cairo), Egypt 19 128 Lagos, Nigeria 24 239 10 New York-Newark, USA 18 604 Ciudad de México (Mexico City), Mexico 23 865 11 Dhaka, Bangladesh 18 237 São Paulo, Brazil 23 444 12 Karachi, Pakistan 17 121 Kinshasa, Democratic Republic of the Congo 19 996 13 Buenos Aires, Argentina 15 334 Kinki M.M.A. (Osaka), Japan 19 976 14 Kolkata (Calcutta), India 14 980 New York-Newark, USA 19 885 15 Istanbul, Turkey 14 365 Kolkata (Calcutta), India 19 092 16 Chongqing, China 13 744 Guangzhou, Guangdong, China 17 574 17 Lagos, Nigeria 13 661 Chongqing, China 17 380 18 Manila, Philippines 13 131 Buenos Aires, Argentina 16 956 19 Guangzhou, Guangdong, China 13 070 Manila, Philippines 16 756 20 Rio de Janeiro, Brazil 12 981 Istanbul, Turkey 16 694 21 Los Angeles-Long Beach-Santa Ana, USA 12 317 Bangalore, India 14 762 22 Moskva (Moscow), Russian Federation 12 260 Tianjin, China 14 655 23 Kinshasa, Democratic Republic of the Congo 12 071 Rio de Janeiro, Brazil 14 174 24 Tianjin, China 11 558 Chennai (Madras), India 13 921</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2.0 1.4 0.3 0.5 China Shaoxing Urban Agglomeration 1 124 2 151 2 841 4.1 2.0 0.2 0.3 China Shenyang Urban Agglomeration 4 562 6 438 7 911 2.2 1.5 0.5 0.8 China Shenzhen Urban Agglomeration 6 550 10 828 12 673 3.1 1.1 0.8 1.4 China Shijiazhuang Urban Agglomeration 1 914 3 370 4 362 3.5 1.8 0.2 0.4 China Suqian Urban Agglomeration 397 1 111 1 591 6.4 2.6 0.1 0.1 China Suzhou, Jiangsu Urban Agglomeration 2 112 5 788 8 098 6.3 2.4 0.4 0.7 China Taian, Shandong Urban Agglomeration 910 1 239 1 541 1.9 1.6 0.1 0.2 China Taichung Urban Agglomeration 978 1 241 1 528 1.5 1.5 0.1 0.2 China Taipei Urban Agglomeration 2 630 2 669 3 116 0.1 1.1 0.2 0.3 China Taiyuan, Shanxi Urban Agglomeration 2 503 3 549 4 396 2.2 1.5 0.3 0.4 China Taizhou, Jiangsu Urban Agglomeration 784 1 211 1 541 2.7 1.7 0.1 0.2 China Taizhou, Zhejiang City Proper 992 1 695 2 189 3.4 1.8 0.1 0.2 China Tangshan, Hebei Urban Agglomeration 1 418 2 853 3 801 4.4 2.0 0.2 0.4 China Tianjin Urban Agglomeration 6 670 11 558 14 655 3.4 1.7 0.8 1.4 China Ürümqi (Wulumqi) Urban Agglomeration 1 807 3 639 4 831 4.4 2.0 0.3 0.5 China Weifang Urban Agglomeration 1 235 2 269 2 973 3.8 1.9 0.2 0.3 China Wenzhou Urban Agglomeration 1 565 3 319 4 336 4.7 1.9 0.2 0.4 China Wuhan Urban Agglomeration 6 638 7 979 9 442 1.2 1.2 0.6 1.0 China Wuhu, Anhui Urban Agglomeration 634 1 495 2 074 5.4 2.3 0.1 0.2 China Wuxi, Jiangsu Urban Agglomeration 1 835 3 109 3 862 3.3 1.5 0.2 0.4 China Xi’an, Shaanxi Urban Agglomeration 3 690 6 220 7 904 3.3 1.7 0.4 0.8 China Xiamen Urban Agglomeration 1 416 4 738 6 911 7.5 2.7 0.3 0.6 China Xiangtan, Hunan Urban Agglomeration 698 1 032 1 311 2.4 1.7 0.1 0.1 14 The World’s Cities in 2016 City population (thousands)</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>India 13 921 25 Paris, France 10 925 Jakarta, Indonesia 13 812 26 Shenzhen, China 10 828 Los Angeles-Long Beach-Santa Ana, USA 13 257 27 Jakarta, Indonesia 10 483 Lahore, Pakistan 13 033 28 Bangalore, India 10 456 Hyderabad, India 12 774 29 London, United Kingdom 10 434 Shenzhen, China 12 673 30 Chennai (Madras), India 10 163 Lima, Peru 12 221 31 Lima, Peru 10 072 Moskva (Moscow), Russian Federation 12 200 32 Bogotá, Colombia 11 966 33 Paris, France 11 803 34 Johannesburg, South Africa 11 573 35 Krung Thep (Bangkok), Thailand 11 528 36 London, United Kingdom 11 467 37 Dar es Salaam, United Republic of Tanzania 10 760 38 Ahmadabad, India 10 527 39 Luanda, Angola 10 429 40 Thành Pho Ho Chí Minh (Ho Chi Minh City), Viet Nam 10 200 41 Chengdu, China 10 104 5The World’s Cities in 2016 The share of the population residing in cities is projected to increase in all regions In Northern America, more than half of the population resided in cities with 500,000 inhabitants or more in 2016 and one in five people lived in a city of 5 million inhabitants or more. Latin America and the Caribbean is the region with the largest proportion of the population concentrated in megacities: of the total population of the region in 2016, 12.7 per cent resided in the five cities with 10 million inhabitants or more and the share in megacities is projected to rise to 14.3 per cent in 2030, as Bogotá crosses the 10 million threshold. In both Africa and Asia, more than half of the population lived in rural areas in 2016, but that share is declining. Between 2016 and 2030, the number of cities with 500,000 inhabitants or more is expected to grow by 80 per cent in Africa and by 30 per cent in Asia. Population distribution by size class of settlement and region, 2016 and 2030 6 The World’s Cities in 2016 Between 2000 and 2016, the world’s cities with 500,000 inhabitants or more grew at an average annual rate of 2.4 per cent. However, 47 of these cities grew more than twice as fast, with average growth in</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>The World’s Cities in 2016 United Nations Data Booklet file:V:\PEP-Section\WUP2014\2016%20Data%20Booklet\Charts%20and%20Images\4_Urbanization_BusanRepublic%20of%20Korea2011UNPhoto_Kibae%20Park_03022015.jpg ii The World’s Cities in 2016 In 2016, an estimated 54.5 per cent of the world’s population lived in urban settlements. By 2030, urban areas are projected to house 60 per cent of people globally and one in every three people will live in cities with at least half a million inhabitants. Understanding the key trends in urbanization likely to unfold over the coming years is crucial to the implementation of the 2030 Agenda for Sustainable Development and for efforts to forge a new framework of ur- ban development during the Habitat III confer- ence scheduled to be held in Quito, Ecuador in October 2016. This data booklet highlights current and future trajectories of populations in cities around the globe, drawing on population estimates and projections published in World Urbanization Prospects: The 2014 Revision. All information is available at www.unpopulation.org. Suggested citation: United Nations, Department of Economic and Social Affairs, Population Di- vision (2016). The World’s Cities in 2016 – Data Booklet (ST/ESA/ SER.A/392). Cover photo: Copyright © UN Photo/Kibae Park 1The World’s Cities in 2016 What is a City? Most people can agree that cities are places where large numbers of people live and work; they are hubs of government, commerce and transportation. But how best to define the geographical limits of a city is a matter of some debate. So far, no standardized international criteria exist for determining the boundaries of a city and often multiple different boundary definitions are available for any given city. One type of definition, sometimes referred to as the “city proper”, describes a city according to an administrative boundary. A second approach, termed the “ur-</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>inhabitants In 2016, 1.7 billion people—23 per cent of the world’s population— lived in a city with at least 1 million inhabitants. By 2030, a projected 27 per cent of people worldwide will be concentrated in cities with at least 1 million inhabitants. Between 2016 and 2030, the population in all city size classes is pro- jected to increase, while the rural population is projected to decline slightly. While rural areas were home to more than 45 per cent of the world’s population in 2016, that proportion is expected to fall to 40 per cent by 2030. A minority of people reside in megacities—500 million, representing 6.8 per cent of the global population in 2016. But, as these cities increase in both size and number, they will become home to a grow- ing share of the population. By 2030, a projected 730 million people will live in cities with at least 10 million inhabitants, representing 8.7 per cent of people globally. World’s population by size class of settlement, 1990-2030 2016 2030 Number of settlements Population (millions) Percentage of world population Number of settlements Population (millions) Percentage of world population Urban .. 4 034 54.5 .. 5 058 60.0 10 million or more 31 500 6.8 41 730 8.7 5 to 10 million 45 308 4.2 63 434 5.2 1 to 5 million 436 861 11.6 558 1 128 13.4 500 000 to 1 million 551 380 5.1 731 509 6.0 Fewer than 500 000 .. 1 985 26.8 .. 2 257 26.8 Rural .. 3 371 45.5 .. 3 367 40.0 World’s population by size class of settlement, 2016 and 2030 4 The World’s Cities in 2016 Most megacities are located in the global South Of the world’s 31 megacities (that is, cities with 10 million inhabitants or more) in 2016, 24 are located in the less developed regions or the “global South”. China alone was home to six megacities in 2016, while India had five. The 10 cities that are projected to be- come megacities between 2016 and 2030 are all located in developing countries.</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
         <is>
           <t>countries. They include: Lahore, Pakistan Hyderabad, India Bogotá, Colombia Johannesburg, South Africa Bangkok, Thailand Dar es Salaam, Tanzania Ahmanabad, India Luanda, Angola Ho Chi Minh City, Viet Nam and Chungdu, China. Despite a projected decline of nearly 1 million inhabitants, Tokyo is ex- pected to remain the world’s largest city in 2030, followed by Delhi, which is projected to add nearly 10 million people between 2016 and 2030. Rank City, Country Population in 2016 (thousands) City, Country Population in 2030 (thousands) 1 Tokyo, Japan 38 140 Tokyo, Japan 37 190 2 Delhi, India 26 454 Delhi, India 36 060 3 Shanghai, China 24 484 Shanghai, China 30 751 4 Mumbai (Bombay), India 21 357 Mumbai (Bombay), India 27 797 5 São Paulo, Brazil 21 297 Beijing, China 27 706 6 Beijing, China 21 240 Dhaka, Bangladesh 27 374 7 Ciudad de México (Mexico City), Mexico 21 157 Karachi, Pakistan 24 838 8 Kinki M.M.A. (Osaka), Japan 20 337 Al-Qahirah (Cairo), Egypt 24 502 9 Al-Qahirah (Cairo), Egypt 19 128 Lagos, Nigeria 24 239 10 New York-Newark, USA 18 604 Ciudad de México (Mexico City), Mexico 23 865 11 Dhaka, Bangladesh 18 237 São Paulo, Brazil 23 444 12 Karachi, Pakistan 17 121 Kinshasa, Democratic Republic of the Congo 19 996 13 Buenos Aires, Argentina 15 334 Kinki M.M.A. (Osaka), Japan 19 976 14 Kolkata (Calcutta), India 14 980 New York-Newark, USA 19 885 15 Istanbul, Turkey 14 365 Kolkata (Calcutta), India 19 092 16 Chongqing, China 13 744 Guangzhou, Guangdong, China 17 574 17 Lagos, Nigeria 13 661 Chongqing, China 17 380 18 Manila, Philippines 13 131 Buenos Aires, Argentina 16 956 19 Guangzhou, Guangdong, China 13 070 Manila, Philippines 16 756 20 Rio de Janeiro, Brazil 12 981 Istanbul, Turkey 16 694 21 Los Angeles-Long Beach-Santa Ana, USA 12 317 Bangalore, India 14 762 22 Moskva (Moscow), Russian Federation 12 260 Tianjin, China 14 655 23 Kinshasa, Democratic Republic of the Congo 12 071 Rio de Janeiro, Brazil 14 174 24 Tianjin, China 11 558 Chennai (Madras), India 13 921</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>India 13 921 25 Paris, France 10 925 Jakarta, Indonesia 13 812 26 Shenzhen, China 10 828 Los Angeles-Long Beach-Santa Ana, USA 13 257 27 Jakarta, Indonesia 10 483 Lahore, Pakistan 13 033 28 Bangalore, India 10 456 Hyderabad, India 12 774 29 London, United Kingdom 10 434 Shenzhen, China 12 673 30 Chennai (Madras), India 10 163 Lima, Peru 12 221 31 Lima, Peru 10 072 Moskva (Moscow), Russian Federation 12 200 32 Bogotá, Colombia 11 966 33 Paris, France 11 803 34 Johannesburg, South Africa 11 573 35 Krung Thep (Bangkok), Thailand 11 528 36 London, United Kingdom 11 467 37 Dar es Salaam, United Republic of Tanzania 10 760 38 Ahmadabad, India 10 527 39 Luanda, Angola 10 429 40 Thành Pho Ho Chí Minh (Ho Chi Minh City), Viet Nam 10 200 41 Chengdu, China 10 104 5The World’s Cities in 2016 The share of the population residing in cities is projected to increase in all regions In Northern America, more than half of the population resided in cities with 500,000 inhabitants or more in 2016 and one in five people lived in a city of 5 million inhabitants or more. Latin America and the Caribbean is the region with the largest proportion of the population concentrated in megacities: of the total population of the region in 2016, 12.7 per cent resided in the five cities with 10 million inhabitants or more and the share in megacities is projected to rise to 14.3 per cent in 2030, as Bogotá crosses the 10 million threshold. In both Africa and Asia, more than half of the population lived in rural areas in 2016, but that share is declining. Between 2016 and 2030, the number of cities with 500,000 inhabitants or more is expected to grow by 80 per cent in Africa and by 30 per cent in Asia. Population distribution by size class of settlement and region, 2016 and 2030 6 The World’s Cities in 2016 Between 2000 and 2016, the world’s cities with 500,000 inhabitants or more grew at an average annual rate of 2.4 per cent. However, 47 of these cities grew more than twice as fast, with average growth in</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>countries. They include: Lahore, Pakistan Hyderabad, India Bogotá, Colombia Johannesburg, South Africa Bangkok, Thailand Dar es Salaam, Tanzania Ahmanabad, India Luanda, Angola Ho Chi Minh City, Viet Nam and Chungdu, China. Despite a projected decline of nearly 1 million inhabitants, Tokyo is ex- pected to remain the world’s largest city in 2030, followed by Delhi, which is projected to add nearly 10 million people between 2016 and 2030. Rank City, Country Population in 2016 (thousands) City, Country Population in 2030 (thousands) 1 Tokyo, Japan 38 140 Tokyo, Japan 37 190 2 Delhi, India 26 454 Delhi, India 36 060 3 Shanghai, China 24 484 Shanghai, China 30 751 4 Mumbai (Bombay), India 21 357 Mumbai (Bombay), India 27 797 5 São Paulo, Brazil 21 297 Beijing, China 27 706 6 Beijing, China 21 240 Dhaka, Bangladesh 27 374 7 Ciudad de México (Mexico City), Mexico 21 157 Karachi, Pakistan 24 838 8 Kinki M.M.A. (Osaka), Japan 20 337 Al-Qahirah (Cairo), Egypt 24 502 9 Al-Qahirah (Cairo), Egypt 19 128 Lagos, Nigeria 24 239 10 New York-Newark, USA 18 604 Ciudad de México (Mexico City), Mexico 23 865 11 Dhaka, Bangladesh 18 237 São Paulo, Brazil 23 444 12 Karachi, Pakistan 17 121 Kinshasa, Democratic Republic of the Congo 19 996 13 Buenos Aires, Argentina 15 334 Kinki M.M.A. (Osaka), Japan 19 976 14 Kolkata (Calcutta), India 14 980 New York-Newark, USA 19 885 15 Istanbul, Turkey 14 365 Kolkata (Calcutta), India 19 092 16 Chongqing, China 13 744 Guangzhou, Guangdong, China 17 574 17 Lagos, Nigeria 13 661 Chongqing, China 17 380 18 Manila, Philippines 13 131 Buenos Aires, Argentina 16 956 19 Guangzhou, Guangdong, China 13 070 Manila, Philippines 16 756 20 Rio de Janeiro, Brazil 12 981 Istanbul, Turkey 16 694 21 Los Angeles-Long Beach-Santa Ana, USA 12 317 Bangalore, India 14 762 22 Moskva (Moscow), Russian Federation 12 260 Tianjin, China 14 655 23 Kinshasa, Democratic Republic of the Congo 12 071 Rio de Janeiro, Brazil 14 174 24 Tianjin, China 11 558 Chennai (Madras), India 13 921</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>India 13 921 25 Paris, France 10 925 Jakarta, Indonesia 13 812 26 Shenzhen, China 10 828 Los Angeles-Long Beach-Santa Ana, USA 13 257 27 Jakarta, Indonesia 10 483 Lahore, Pakistan 13 033 28 Bangalore, India 10 456 Hyderabad, India 12 774 29 London, United Kingdom 10 434 Shenzhen, China 12 673 30 Chennai (Madras), India 10 163 Lima, Peru 12 221 31 Lima, Peru 10 072 Moskva (Moscow), Russian Federation 12 200 32 Bogotá, Colombia 11 966 33 Paris, France 11 803 34 Johannesburg, South Africa 11 573 35 Krung Thep (Bangkok), Thailand 11 528 36 London, United Kingdom 11 467 37 Dar es Salaam, United Republic of Tanzania 10 760 38 Ahmadabad, India 10 527 39 Luanda, Angola 10 429 40 Thành Pho Ho Chí Minh (Ho Chi Minh City), Viet Nam 10 200 41 Chengdu, China 10 104 5The World’s Cities in 2016 The share of the population residing in cities is projected to increase in all regions In Northern America, more than half of the population resided in cities with 500,000 inhabitants or more in 2016 and one in five people lived in a city of 5 million inhabitants or more. Latin America and the Caribbean is the region with the largest proportion of the population concentrated in megacities: of the total population of the region in 2016, 12.7 per cent resided in the five cities with 10 million inhabitants or more and the share in megacities is projected to rise to 14.3 per cent in 2030, as Bogotá crosses the 10 million threshold. In both Africa and Asia, more than half of the population lived in rural areas in 2016, but that share is declining. Between 2016 and 2030, the number of cities with 500,000 inhabitants or more is expected to grow by 80 per cent in Africa and by 30 per cent in Asia. Population distribution by size class of settlement and region, 2016 and 2030 6 The World’s Cities in 2016 Between 2000 and 2016, the world’s cities with 500,000 inhabitants or more grew at an average annual rate of 2.4 per cent. However, 47 of these cities grew more than twice as fast, with average growth in</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>countries. They include: Lahore, Pakistan Hyderabad, India Bogotá, Colombia Johannesburg, South Africa Bangkok, Thailand Dar es Salaam, Tanzania Ahmanabad, India Luanda, Angola Ho Chi Minh City, Viet Nam and Chungdu, China. Despite a projected decline of nearly 1 million inhabitants, Tokyo is ex- pected to remain the world’s largest city in 2030, followed by Delhi, which is projected to add nearly 10 million people between 2016 and 2030. Rank City, Country Population in 2016 (thousands) City, Country Population in 2030 (thousands) 1 Tokyo, Japan 38 140 Tokyo, Japan 37 190 2 Delhi, India 26 454 Delhi, India 36 060 3 Shanghai, China 24 484 Shanghai, China 30 751 4 Mumbai (Bombay), India 21 357 Mumbai (Bombay), India 27 797 5 São Paulo, Brazil 21 297 Beijing, China 27 706 6 Beijing, China 21 240 Dhaka, Bangladesh 27 374 7 Ciudad de México (Mexico City), Mexico 21 157 Karachi, Pakistan 24 838 8 Kinki M.M.A. (Osaka), Japan 20 337 Al-Qahirah (Cairo), Egypt 24 502 9 Al-Qahirah (Cairo), Egypt 19 128 Lagos, Nigeria 24 239 10 New York-Newark, USA 18 604 Ciudad de México (Mexico City), Mexico 23 865 11 Dhaka, Bangladesh 18 237 São Paulo, Brazil 23 444 12 Karachi, Pakistan 17 121 Kinshasa, Democratic Republic of the Congo 19 996 13 Buenos Aires, Argentina 15 334 Kinki M.M.A. (Osaka), Japan 19 976 14 Kolkata (Calcutta), India 14 980 New York-Newark, USA 19 885 15 Istanbul, Turkey 14 365 Kolkata (Calcutta), India 19 092 16 Chongqing, China 13 744 Guangzhou, Guangdong, China 17 574 17 Lagos, Nigeria 13 661 Chongqing, China 17 380 18 Manila, Philippines 13 131 Buenos Aires, Argentina 16 956 19 Guangzhou, Guangdong, China 13 070 Manila, Philippines 16 756 20 Rio de Janeiro, Brazil 12 981 Istanbul, Turkey 16 694 21 Los Angeles-Long Beach-Santa Ana, USA 12 317 Bangalore, India 14 762 22 Moskva (Moscow), Russian Federation 12 260 Tianjin, China 14 655 23 Kinshasa, Democratic Republic of the Congo 12 071 Rio de Janeiro, Brazil 14 174 24 Tianjin, China 11 558 Chennai (Madras), India 13 921</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>average growth in excess of 6 per cent per year. Of these, 6 are located in Africa, 40 in Asia (20 in China alone), and 1 in Northern America. Among the fast- est growing cities, 31 (nearly two thirds) have a long history of rapid population growth, with average annual growth rates above 6 per cent for the period 1980-2000 as well. None of the 47 fastest growing cities had a population greater than 5 million in 2000, only 4 had between 1 and 5 million inhabitants, and 43 had fewer than 1 million inhabitants. Most of the world’s fastest growing cities are located in Asia and Africa Cities where population declined between 2000 and 2016 Population decline in some cities occurred in response to a natu- ral disaster. This has been the case in the United States city of New Orleans, which lost population after Hurricane Katrina in 2005, and in Sendai, Japan, following the 2011 earthquake and tsunami. Economic contraction has also contributed to popula- tion decline in places such as Buffalo and Detroit, concurrent with the loss of industry and jobs in those cities. In most cases, however, city population decline has been associ- ated not with crises, but rather with persistent low fertility rates, which have contributed to stagnating or declining total popula- tion sizes in some countries, particularly in Europe. The 55 cities with declining populations were home to 70 million people in 2016. Growth rate of the world’s cities, 2000-2016 * Out of the 1,063 cities with 500,000 inhabitants or more in 2016. Fifty-five cities have experienced population decline since 2000* − 2 0 2 4 6 8 1 0 1 2 A ve ra g e a n n u a l ra te o f c h a n g e ( p e rc e n ta g e ) Africa Asia Europe Latin America and the Caribbean Northern America Oceania City size class 10 million or more 5 to 10 million 1 to 5 million 500 000 to 1 million 7The World’s Cities in 2016 In 28 countries or areas, more than 40 per cent of the urban population is</t>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Southern Europe Greece Athínai (Athens) Urban Agglomeration 3 179 3 046 3 169 -0.3 0.3 27.4 35.0 Italy Milano (Milan) Metropolitan area 2 985 3 104 3 162 0.2 0.1 5.1 7.3 Italy Napoli (Naples) Metropolitan area 2 232 2 198 2 226 -0.1 0.1 3.6 5.2 Italy Roma (Rome) Metropolitan area 3 385 3 738 3 842 0.6 0.2 6.1 8.8 Italy Torino (Turin) Metropolitan area 1 694 1 769 1 825 0.3 0.2 2.9 4.2 Portugal Lisboa (Lisbon) Metropolitan area 2 672 2 902 3 192 0.5 0.7 27.4 42.7 Portugal Porto Metropolitan area 1 254 1 304 1 443 0.2 0.7 12.3 19.2 Serbia Beograd (Belgrade) Urban Agglomeration 1 122 1 183 1 196 0.3 0.1 12.6 22.7 Spain Barcelona City Proper 4 355 5 309 5 685 1.2 0.5 11.2 14.1 Spain Madrid City Proper 5 014 6 264 6 707 1.4 0.5 13.2 16.6 Western Europe Austria Wien (Vienna) City Proper 1 549 1 763 1 959 0.8 0.8 20.5 31.1 Belgium Bruxelles-Brussel Metropolitan area 1 792 2 061 2 203 0.9 0.5 18.4 18.8 France Lille Urban Agglomeration 1 002 1 030 1 142 0.2 0.7 1.6 2.0 France Lyon Urban Agglomeration 1 443 1 622 1 814 0.7 0.8 2.5 3.1 France Marseille-Aix-en-Provence Urban Agglomeration 1 474 1 616 1 798 0.6 0.8 2.5 3.1 France Paris Urban Agglomeration 9 737 10 925 11 803 0.7 0.6 16.7 21.0 Germany Berlin City Proper 3 384 3 578 3 658 0.3 0.2 4.3 5.7 Germany Hamburg City Proper 1 710 1 839 1 906 0.5 0.3 2.2 3.0 Germany Köln (Cologne) City Proper 963 1 042 1 095 0.5 0.4 1.3 1.7 Germany München (Munich) City Proper 1 202 1 454 1 548 1.2 0.4 1.8 2.3 22 The World’s Cities in 2016 City population (thousands) Average annual rate of change (percentage) City population as a proportion of the country or area’s total or urban population in 2016 (percentage)</t>
         </is>
       </c>
     </row>

</xml_diff>